<commit_message>
Minor refactorings, mainly storing the start and goal as member variables and extracting some code into methods to make it cleaner.
</commit_message>
<xml_diff>
--- a/Data/results.xlsx
+++ b/Data/results.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,7 +369,7 @@
         <v>42</v>
       </c>
       <c r="E1" t="n">
-        <v>0.5520288944244385</v>
+        <v>0.5649590492248535</v>
       </c>
       <c r="F1" t="n">
         <v>123</v>
@@ -382,6 +382,37 @@
       </c>
       <c r="I1" t="n">
         <v>124</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ResultsA3.csv</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>42</v>
+      </c>
+      <c r="E2" t="n">
+        <v>29.99599480628967</v>
+      </c>
+      <c r="F2" t="n">
+        <v>123</v>
+      </c>
+      <c r="G2" t="n">
+        <v>124462</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>